<commit_message>
Classwork as of 12/4/2024
</commit_message>
<xml_diff>
--- a/Copy of ButlerHighway.xlsx
+++ b/Copy of ButlerHighway.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5b61916b0c219c5/Desktop/QMBE_1320_Laura_Hardy/QMBE1320_Laura_Hardy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{95155E4F-66DA-4BE9-8944-C26929C9D983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04ECD445-3383-4FA1-A53D-9F05BE76EDB5}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{95155E4F-66DA-4BE9-8944-C26929C9D983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BAC789C-38ED-4408-B87A-35595EC33732}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Assignment</t>
   </si>
@@ -123,12 +121,6 @@
   </si>
   <si>
     <t>Upper 95.0%</t>
-  </si>
-  <si>
-    <t>PROBABILITY OUTPUT</t>
-  </si>
-  <si>
-    <t>Percentile</t>
   </si>
 </sst>
 </file>
@@ -253,2009 +245,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Normal Probability Plot</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$26:$A$324</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="299"/>
-                <c:pt idx="0">
-                  <c:v>0.16722408026755853</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50167224080267558</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.83612040133779264</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1705685618729098</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5050167224080266</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.8394648829431439</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1739130434782608</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.508361204013378</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8428093645484949</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.1772575250836117</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.511705685618729</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.8461538461538463</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.1806020066889635</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.5150501672240804</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.8494983277591981</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.1839464882943149</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.5183946488294318</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.8528428093645486</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.1872909698996654</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6.5217391304347831</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.8561872909699</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.1906354515050168</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.5250836120401345</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.8595317725752514</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8.1939799331103682</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8.5284280936454859</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.8628762541806019</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.1973244147157196</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.5317725752508373</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9.8662207357859533</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10.200668896321071</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10.535117056856187</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>10.869565217391305</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>11.204013377926422</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11.538461538461538</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>11.872909698996656</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>12.207357859531772</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>12.54180602006689</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>12.876254180602007</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>13.210702341137123</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>13.545150501672241</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>13.879598662207359</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>14.214046822742475</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>14.548494983277592</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>14.88294314381271</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>15.217391304347826</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>15.551839464882944</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>15.88628762541806</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>16.220735785953178</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>16.555183946488295</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>16.889632107023413</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>17.224080267558527</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>17.558528428093645</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>17.892976588628763</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>18.22742474916388</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>18.561872909698998</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>18.896321070234116</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>19.23076923076923</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>19.565217391304348</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>19.899665551839465</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>20.234113712374583</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>20.568561872909701</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>20.903010033444815</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>21.237458193979933</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>21.57190635451505</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>21.906354515050168</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>22.240802675585286</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>22.5752508361204</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>22.909698996655518</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>23.244147157190636</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>23.578595317725753</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>23.913043478260871</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>24.247491638795985</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>24.581939799331103</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>24.916387959866221</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>25.250836120401338</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>25.585284280936456</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>25.919732441471574</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>26.254180602006688</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>26.588628762541806</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>26.923076923076923</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>27.257525083612041</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>27.591973244147159</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>27.926421404682273</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>28.260869565217391</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>28.595317725752508</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>28.929765886287626</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>29.264214046822744</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>29.598662207357862</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>29.933110367892976</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>30.267558528428093</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>30.602006688963211</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>30.936454849498329</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>31.270903010033447</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>31.605351170568561</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>31.939799331103679</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>32.274247491638796</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>32.608695652173914</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>32.943143812709032</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>33.277591973244149</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>33.612040133779267</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>33.946488294314385</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>34.280936454849495</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>34.615384615384613</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>34.949832775919731</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>35.284280936454849</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>35.618729096989966</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>35.953177257525084</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>36.287625418060202</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>36.62207357859532</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>36.956521739130437</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>37.290969899665555</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>37.625418060200673</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>37.959866220735783</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>38.294314381270901</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>38.628762541806019</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>38.963210702341136</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>39.297658862876254</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>39.632107023411372</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>39.96655518394649</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>40.301003344481607</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>40.635451505016725</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>40.969899665551843</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>41.304347826086953</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>41.638795986622071</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>41.973244147157189</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>42.307692307692307</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>42.642140468227424</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>42.976588628762542</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>43.31103678929766</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>43.645484949832777</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>43.979933110367895</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>44.314381270903013</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>44.648829431438131</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>44.983277591973241</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>45.317725752508359</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>45.652173913043477</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>45.986622073578594</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>46.321070234113712</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>46.65551839464883</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>46.989966555183948</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>47.324414715719065</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>47.658862876254183</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>47.993311036789301</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>48.327759197324411</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>48.662207357859529</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>48.996655518394647</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>49.331103678929765</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>49.665551839464882</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>50.334448160535118</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>50.668896321070235</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>51.003344481605353</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>51.337792642140471</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>51.672240802675589</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>52.006688963210699</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>52.341137123745817</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>52.675585284280935</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>53.010033444816052</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>53.34448160535117</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>53.678929765886288</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>54.013377926421406</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>54.347826086956523</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>54.682274247491641</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>55.016722408026759</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>55.351170568561876</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>55.685618729096987</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>56.020066889632105</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>56.354515050167223</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>56.68896321070234</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>57.023411371237458</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>57.357859531772576</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>57.692307692307693</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>58.026755852842811</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>58.361204013377929</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>58.695652173913047</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>59.030100334448164</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>59.364548494983275</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>59.698996655518393</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>60.03344481605351</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>60.367892976588628</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>60.702341137123746</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>61.036789297658864</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>61.371237458193981</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>61.705685618729099</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>62.040133779264217</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>62.374581939799334</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>62.709030100334445</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>63.043478260869563</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>63.37792642140468</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>63.712374581939798</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>64.046822742474916</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>64.381270903010034</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>64.715719063545151</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>65.050167224080269</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>65.384615384615387</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>65.719063545150505</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>66.053511705685622</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>66.38795986622074</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>66.722408026755858</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>67.056856187290975</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>67.391304347826093</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>67.725752508361211</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>68.060200668896314</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>68.394648829431432</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>68.72909698996655</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>69.063545150501668</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>69.397993311036785</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>69.732441471571903</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>70.066889632107021</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>70.401337792642138</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>70.735785953177256</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>71.070234113712374</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>71.404682274247492</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>71.739130434782609</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>72.073578595317727</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>72.408026755852845</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>72.742474916387962</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>73.07692307692308</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>73.411371237458198</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>73.745819397993316</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>74.080267558528433</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>74.414715719063551</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>74.749163879598669</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>75.083612040133787</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>75.41806020066889</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>75.752508361204008</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>76.086956521739125</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>76.421404682274243</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>76.755852842809361</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>77.090301003344479</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>77.424749163879596</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>77.759197324414714</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>78.093645484949832</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>78.42809364548495</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>78.762541806020067</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>79.096989966555185</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>79.431438127090303</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>79.76588628762542</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>80.100334448160538</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>80.434782608695656</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>80.769230769230774</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>81.103678929765891</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>81.438127090301009</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>81.772575250836127</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>82.107023411371244</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>82.441471571906348</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>82.775919732441466</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>83.110367892976583</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>83.444816053511701</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>83.779264214046819</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>84.113712374581937</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>84.448160535117054</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>84.782608695652172</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>85.11705685618729</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>85.451505016722408</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>85.785953177257525</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>86.120401337792643</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>86.454849498327761</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>86.789297658862878</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>87.123745819397996</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>87.458193979933114</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>87.792642140468232</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>88.127090301003349</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>88.461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>88.795986622073585</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>89.130434782608702</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>89.464882943143806</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>89.799331103678924</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>90.133779264214041</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>90.468227424749159</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>90.802675585284277</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>91.137123745819395</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>91.471571906354512</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>91.80602006688963</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>92.140468227424748</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>92.474916387959865</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>92.809364548494983</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>93.143812709030101</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>93.478260869565219</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>93.812709030100336</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>94.147157190635454</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>94.481605351170572</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>94.81605351170569</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>95.150501672240807</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>95.484949832775925</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>95.819397993311043</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>96.15384615384616</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>96.488294314381264</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>96.822742474916382</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>97.157190635451499</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>97.491638795986617</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>97.826086956521735</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>98.160535117056853</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>98.49498327759197</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>98.829431438127088</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>99.163879598662206</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>99.498327759197323</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>99.832775919732441</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$26:$B$324</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="299"/>
-                <c:pt idx="0">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4.9000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.9000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.4</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.4</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>6.6</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>8.1</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>8.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>9.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>9.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>10.1</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>10.4</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>10.6</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>10.6</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>10.8</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>10.9</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>11.1</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>11.2</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>11.2</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>11.3</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>11.3</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>11.7</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>12.2</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>12.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-85D2-4009-8AE5-651F93E1D340}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1212797247"/>
-        <c:axId val="1212789567"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1212797247"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sample Percentile</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1212789567"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1212789567"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>9.3</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1212797247"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286BF4FB-AC19-1D38-F3B4-BD12CA4C7CA0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2547,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -7979,17 +5968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DF4CCE-CFF5-4F69-91E7-499A28A05DA8}">
-  <dimension ref="A1:I324"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF1F6CE-802B-41BE-B84B-40C1BD881019}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8008,7 +5994,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="8">
-        <v>0.90375158314757653</v>
+        <v>0.94010722815394976</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -8016,7 +6002,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="8">
-        <v>0.816766924041751</v>
+        <v>0.88380160042730249</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -8024,7 +6010,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="8">
-        <v>0.81552886271770886</v>
+        <v>0.88262391394514672</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -8032,7 +6018,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="8">
-        <v>0.83117622196948082</v>
+        <v>0.66310642616384541</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8040,7 +6026,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="9">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8071,19 +6057,19 @@
         <v>13</v>
       </c>
       <c r="B12" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="8">
-        <v>911.53259322819963</v>
+        <v>989.94900080374248</v>
       </c>
       <c r="D12" s="8">
-        <v>455.76629661409982</v>
+        <v>329.98300026791418</v>
       </c>
       <c r="E12" s="8">
-        <v>659.71443270276666</v>
+        <v>750.45575695963805</v>
       </c>
       <c r="F12" s="8">
-        <v>8.4056845737967337E-110</v>
+        <v>5.7766280211206763E-138</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -8094,10 +6080,10 @@
         <v>296</v>
       </c>
       <c r="C13" s="8">
-        <v>204.49275794236809</v>
+        <v>130.15419919625705</v>
       </c>
       <c r="D13" s="8">
-        <v>0.69085391196745971</v>
+        <v>0.43971013241978735</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -8107,10 +6093,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C14" s="9">
-        <v>1116.0253511705678</v>
+        <v>1120.1031999999996</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -8149,2523 +6135,118 @@
         <v>16</v>
       </c>
       <c r="B17" s="8">
-        <v>0.12218615239561714</v>
+        <v>-0.33022930443400722</v>
       </c>
       <c r="C17" s="8">
-        <v>0.20597439980443655</v>
+        <v>0.16767792520172056</v>
       </c>
       <c r="D17" s="8">
-        <v>0.59321038202624898</v>
+        <v>-1.9694262320859079</v>
       </c>
       <c r="E17" s="8">
-        <v>0.55349334463011446</v>
+        <v>4.9836509835018916E-2</v>
       </c>
       <c r="F17" s="8">
-        <v>-0.28317367602024052</v>
+        <v>-0.66022126000436376</v>
       </c>
       <c r="G17" s="8">
-        <v>0.52754598081147486</v>
+        <v>-2.373488636507326E-4</v>
       </c>
       <c r="H17" s="8">
-        <v>-0.28317367602024052</v>
+        <v>-0.66022126000436376</v>
       </c>
       <c r="I17" s="8">
-        <v>0.52754598081147486</v>
+        <v>-2.373488636507326E-4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
-        <v>100</v>
+      <c r="A18" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>6.7260462159155113E-2</v>
+        <v>6.7220302345733784E-2</v>
       </c>
       <c r="C18" s="8">
-        <v>2.4677625447460366E-3</v>
+        <v>1.961419541553142E-3</v>
       </c>
       <c r="D18" s="8">
-        <v>27.255645930097806</v>
+        <v>34.271251469487076</v>
       </c>
       <c r="E18" s="8">
-        <v>1.0921269775588899E-82</v>
+        <v>4.7851855909105959E-105</v>
       </c>
       <c r="F18" s="8">
-        <v>6.2403878998048182E-2</v>
+        <v>6.336020764673049E-2</v>
       </c>
       <c r="G18" s="8">
-        <v>7.2117045320262044E-2</v>
+        <v>7.1080397044737079E-2</v>
       </c>
       <c r="H18" s="8">
-        <v>6.2403878998048182E-2</v>
+        <v>6.336020764673049E-2</v>
       </c>
       <c r="I18" s="8">
-        <v>7.2117045320262044E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
+        <v>7.1080397044737079E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.67351584017674304</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2.3619992565204057E-2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>28.514650811911654</v>
+      </c>
+      <c r="E19" s="8">
+        <v>6.7479678991178509E-87</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.62703144142376399</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.72000023892972209</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.62703144142376399</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.72000023892972209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="9">
-        <v>0.69017435887058654</v>
-      </c>
-      <c r="C19" s="9">
-        <v>2.956789807366763E-2</v>
-      </c>
-      <c r="D19" s="9">
-        <v>23.34201630264808</v>
-      </c>
-      <c r="E19" s="9">
-        <v>4.4896456829021183E-69</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0.6319844182704959</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0.74836429947067717</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0.6319844182704959</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0.74836429947067717</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="10">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>0.16722408026755853</v>
-      </c>
-      <c r="B26" s="8">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>0.50167224080267558</v>
-      </c>
-      <c r="B27" s="8">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>0.83612040133779264</v>
-      </c>
-      <c r="B28" s="8">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
-        <v>1.1705685618729098</v>
-      </c>
-      <c r="B29" s="8">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
-        <v>1.5050167224080266</v>
-      </c>
-      <c r="B30" s="8">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
-        <v>1.8394648829431439</v>
-      </c>
-      <c r="B31" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
-        <v>2.1739130434782608</v>
-      </c>
-      <c r="B32" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
-        <v>2.508361204013378</v>
-      </c>
-      <c r="B33" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>2.8428093645484949</v>
-      </c>
-      <c r="B34" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
-        <v>3.1772575250836117</v>
-      </c>
-      <c r="B35" s="8">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>3.511705685618729</v>
-      </c>
-      <c r="B36" s="8">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
-        <v>3.8461538461538463</v>
-      </c>
-      <c r="B37" s="8">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
-        <v>4.1806020066889635</v>
-      </c>
-      <c r="B38" s="8">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
-        <v>4.5150501672240804</v>
-      </c>
-      <c r="B39" s="8">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
-        <v>4.8494983277591981</v>
-      </c>
-      <c r="B40" s="8">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
-        <v>5.1839464882943149</v>
-      </c>
-      <c r="B41" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="8">
-        <v>5.5183946488294318</v>
-      </c>
-      <c r="B42" s="8">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
-        <v>5.8528428093645486</v>
-      </c>
-      <c r="B43" s="8">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="8">
-        <v>6.1872909698996654</v>
-      </c>
-      <c r="B44" s="8">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
-        <v>6.5217391304347831</v>
-      </c>
-      <c r="B45" s="8">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
-        <v>6.8561872909699</v>
-      </c>
-      <c r="B46" s="8">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
-        <v>7.1906354515050168</v>
-      </c>
-      <c r="B47" s="8">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="8">
-        <v>7.5250836120401345</v>
-      </c>
-      <c r="B48" s="8">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
-        <v>7.8595317725752514</v>
-      </c>
-      <c r="B49" s="8">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="8">
-        <v>8.1939799331103682</v>
-      </c>
-      <c r="B50" s="8">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="8">
-        <v>8.5284280936454859</v>
-      </c>
-      <c r="B51" s="8">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="8">
-        <v>8.8628762541806019</v>
-      </c>
-      <c r="B52" s="8">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
-        <v>9.1973244147157196</v>
-      </c>
-      <c r="B53" s="8">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="8">
-        <v>9.5317725752508373</v>
-      </c>
-      <c r="B54" s="8">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
-        <v>9.8662207357859533</v>
-      </c>
-      <c r="B55" s="8">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="8">
-        <v>10.200668896321071</v>
-      </c>
-      <c r="B56" s="8">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
-        <v>10.535117056856187</v>
-      </c>
-      <c r="B57" s="8">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="8">
-        <v>10.869565217391305</v>
-      </c>
-      <c r="B58" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="8">
-        <v>11.204013377926422</v>
-      </c>
-      <c r="B59" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="8">
-        <v>11.538461538461538</v>
-      </c>
-      <c r="B60" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
-        <v>11.872909698996656</v>
-      </c>
-      <c r="B61" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="8">
-        <v>12.207357859531772</v>
-      </c>
-      <c r="B62" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="8">
-        <v>12.54180602006689</v>
-      </c>
-      <c r="B63" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="8">
-        <v>12.876254180602007</v>
-      </c>
-      <c r="B64" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="8">
-        <v>13.210702341137123</v>
-      </c>
-      <c r="B65" s="8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="8">
-        <v>13.545150501672241</v>
-      </c>
-      <c r="B66" s="8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="8">
-        <v>13.879598662207359</v>
-      </c>
-      <c r="B67" s="8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="8">
-        <v>14.214046822742475</v>
-      </c>
-      <c r="B68" s="8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="8">
-        <v>14.548494983277592</v>
-      </c>
-      <c r="B69" s="8">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="8">
-        <v>14.88294314381271</v>
-      </c>
-      <c r="B70" s="8">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="8">
-        <v>15.217391304347826</v>
-      </c>
-      <c r="B71" s="8">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="8">
-        <v>15.551839464882944</v>
-      </c>
-      <c r="B72" s="8">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="8">
-        <v>15.88628762541806</v>
-      </c>
-      <c r="B73" s="8">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="8">
-        <v>16.220735785953178</v>
-      </c>
-      <c r="B74" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="8">
-        <v>16.555183946488295</v>
-      </c>
-      <c r="B75" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="8">
-        <v>16.889632107023413</v>
-      </c>
-      <c r="B76" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="8">
-        <v>17.224080267558527</v>
-      </c>
-      <c r="B77" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="8">
-        <v>17.558528428093645</v>
-      </c>
-      <c r="B78" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="8">
-        <v>17.892976588628763</v>
-      </c>
-      <c r="B79" s="8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="8">
-        <v>18.22742474916388</v>
-      </c>
-      <c r="B80" s="8">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
-        <v>18.561872909698998</v>
-      </c>
-      <c r="B81" s="8">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="8">
-        <v>18.896321070234116</v>
-      </c>
-      <c r="B82" s="8">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="8">
-        <v>19.23076923076923</v>
-      </c>
-      <c r="B83" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="8">
-        <v>19.565217391304348</v>
-      </c>
-      <c r="B84" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="8">
-        <v>19.899665551839465</v>
-      </c>
-      <c r="B85" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="8">
-        <v>20.234113712374583</v>
-      </c>
-      <c r="B86" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="8">
-        <v>20.568561872909701</v>
-      </c>
-      <c r="B87" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="8">
-        <v>20.903010033444815</v>
-      </c>
-      <c r="B88" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="8">
-        <v>21.237458193979933</v>
-      </c>
-      <c r="B89" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="8">
-        <v>21.57190635451505</v>
-      </c>
-      <c r="B90" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="8">
-        <v>21.906354515050168</v>
-      </c>
-      <c r="B91" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="8">
-        <v>22.240802675585286</v>
-      </c>
-      <c r="B92" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="8">
-        <v>22.5752508361204</v>
-      </c>
-      <c r="B93" s="8">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="8">
-        <v>22.909698996655518</v>
-      </c>
-      <c r="B94" s="8">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="8">
-        <v>23.244147157190636</v>
-      </c>
-      <c r="B95" s="8">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="8">
-        <v>23.578595317725753</v>
-      </c>
-      <c r="B96" s="8">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="8">
-        <v>23.913043478260871</v>
-      </c>
-      <c r="B97" s="8">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="8">
-        <v>24.247491638795985</v>
-      </c>
-      <c r="B98" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="8">
-        <v>24.581939799331103</v>
-      </c>
-      <c r="B99" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="8">
-        <v>24.916387959866221</v>
-      </c>
-      <c r="B100" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="8">
-        <v>25.250836120401338</v>
-      </c>
-      <c r="B101" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="8">
-        <v>25.585284280936456</v>
-      </c>
-      <c r="B102" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="8">
-        <v>25.919732441471574</v>
-      </c>
-      <c r="B103" s="8">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="8">
-        <v>26.254180602006688</v>
-      </c>
-      <c r="B104" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="8">
-        <v>26.588628762541806</v>
-      </c>
-      <c r="B105" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="8">
-        <v>26.923076923076923</v>
-      </c>
-      <c r="B106" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="8">
-        <v>27.257525083612041</v>
-      </c>
-      <c r="B107" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="8">
-        <v>27.591973244147159</v>
-      </c>
-      <c r="B108" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="8">
-        <v>27.926421404682273</v>
-      </c>
-      <c r="B109" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="8">
-        <v>28.260869565217391</v>
-      </c>
-      <c r="B110" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="8">
-        <v>28.595317725752508</v>
-      </c>
-      <c r="B111" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="8">
-        <v>28.929765886287626</v>
-      </c>
-      <c r="B112" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="8">
-        <v>29.264214046822744</v>
-      </c>
-      <c r="B113" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="8">
-        <v>29.598662207357862</v>
-      </c>
-      <c r="B114" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="8">
-        <v>29.933110367892976</v>
-      </c>
-      <c r="B115" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="8">
-        <v>30.267558528428093</v>
-      </c>
-      <c r="B116" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="8">
-        <v>30.602006688963211</v>
-      </c>
-      <c r="B117" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="8">
-        <v>30.936454849498329</v>
-      </c>
-      <c r="B118" s="8">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="8">
-        <v>31.270903010033447</v>
-      </c>
-      <c r="B119" s="8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="8">
-        <v>31.605351170568561</v>
-      </c>
-      <c r="B120" s="8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="8">
-        <v>31.939799331103679</v>
-      </c>
-      <c r="B121" s="8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="8">
-        <v>32.274247491638796</v>
-      </c>
-      <c r="B122" s="8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="8">
-        <v>32.608695652173914</v>
-      </c>
-      <c r="B123" s="8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="8">
-        <v>32.943143812709032</v>
-      </c>
-      <c r="B124" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="8">
-        <v>33.277591973244149</v>
-      </c>
-      <c r="B125" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="8">
-        <v>33.612040133779267</v>
-      </c>
-      <c r="B126" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="8">
-        <v>33.946488294314385</v>
-      </c>
-      <c r="B127" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="8">
-        <v>34.280936454849495</v>
-      </c>
-      <c r="B128" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="8">
-        <v>34.615384615384613</v>
-      </c>
-      <c r="B129" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="8">
-        <v>34.949832775919731</v>
-      </c>
-      <c r="B130" s="8">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="8">
-        <v>35.284280936454849</v>
-      </c>
-      <c r="B131" s="8">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="8">
-        <v>35.618729096989966</v>
-      </c>
-      <c r="B132" s="8">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="8">
-        <v>35.953177257525084</v>
-      </c>
-      <c r="B133" s="8">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="8">
-        <v>36.287625418060202</v>
-      </c>
-      <c r="B134" s="8">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="8">
-        <v>36.62207357859532</v>
-      </c>
-      <c r="B135" s="8">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="8">
-        <v>36.956521739130437</v>
-      </c>
-      <c r="B136" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="8">
-        <v>37.290969899665555</v>
-      </c>
-      <c r="B137" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="8">
-        <v>37.625418060200673</v>
-      </c>
-      <c r="B138" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="8">
-        <v>37.959866220735783</v>
-      </c>
-      <c r="B139" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="8">
-        <v>38.294314381270901</v>
-      </c>
-      <c r="B140" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="8">
-        <v>38.628762541806019</v>
-      </c>
-      <c r="B141" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="8">
-        <v>38.963210702341136</v>
-      </c>
-      <c r="B142" s="8">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="8">
-        <v>39.297658862876254</v>
-      </c>
-      <c r="B143" s="8">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="8">
-        <v>39.632107023411372</v>
-      </c>
-      <c r="B144" s="8">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="8">
-        <v>39.96655518394649</v>
-      </c>
-      <c r="B145" s="8">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="8">
-        <v>40.301003344481607</v>
-      </c>
-      <c r="B146" s="8">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="8">
-        <v>40.635451505016725</v>
-      </c>
-      <c r="B147" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="8">
-        <v>40.969899665551843</v>
-      </c>
-      <c r="B148" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="8">
-        <v>41.304347826086953</v>
-      </c>
-      <c r="B149" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="8">
-        <v>41.638795986622071</v>
-      </c>
-      <c r="B150" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="8">
-        <v>41.973244147157189</v>
-      </c>
-      <c r="B151" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="8">
-        <v>42.307692307692307</v>
-      </c>
-      <c r="B152" s="8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="8">
-        <v>42.642140468227424</v>
-      </c>
-      <c r="B153" s="8">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="8">
-        <v>42.976588628762542</v>
-      </c>
-      <c r="B154" s="8">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="8">
-        <v>43.31103678929766</v>
-      </c>
-      <c r="B155" s="8">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="8">
-        <v>43.645484949832777</v>
-      </c>
-      <c r="B156" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="8">
-        <v>43.979933110367895</v>
-      </c>
-      <c r="B157" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="8">
-        <v>44.314381270903013</v>
-      </c>
-      <c r="B158" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="8">
-        <v>44.648829431438131</v>
-      </c>
-      <c r="B159" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="8">
-        <v>44.983277591973241</v>
-      </c>
-      <c r="B160" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="8">
-        <v>45.317725752508359</v>
-      </c>
-      <c r="B161" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="8">
-        <v>45.652173913043477</v>
-      </c>
-      <c r="B162" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="8">
-        <v>45.986622073578594</v>
-      </c>
-      <c r="B163" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="8">
-        <v>46.321070234113712</v>
-      </c>
-      <c r="B164" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="8">
-        <v>46.65551839464883</v>
-      </c>
-      <c r="B165" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="8">
-        <v>46.989966555183948</v>
-      </c>
-      <c r="B166" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="8">
-        <v>47.324414715719065</v>
-      </c>
-      <c r="B167" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="8">
-        <v>47.658862876254183</v>
-      </c>
-      <c r="B168" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="8">
-        <v>47.993311036789301</v>
-      </c>
-      <c r="B169" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="8">
-        <v>48.327759197324411</v>
-      </c>
-      <c r="B170" s="8">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="8">
-        <v>48.662207357859529</v>
-      </c>
-      <c r="B171" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="8">
-        <v>48.996655518394647</v>
-      </c>
-      <c r="B172" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="8">
-        <v>49.331103678929765</v>
-      </c>
-      <c r="B173" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="8">
-        <v>49.665551839464882</v>
-      </c>
-      <c r="B174" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="8">
-        <v>50</v>
-      </c>
-      <c r="B175" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="8">
-        <v>50.334448160535118</v>
-      </c>
-      <c r="B176" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="8">
-        <v>50.668896321070235</v>
-      </c>
-      <c r="B177" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="8">
-        <v>51.003344481605353</v>
-      </c>
-      <c r="B178" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="8">
-        <v>51.337792642140471</v>
-      </c>
-      <c r="B179" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="8">
-        <v>51.672240802675589</v>
-      </c>
-      <c r="B180" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="8">
-        <v>52.006688963210699</v>
-      </c>
-      <c r="B181" s="8">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="8">
-        <v>52.341137123745817</v>
-      </c>
-      <c r="B182" s="8">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="8">
-        <v>52.675585284280935</v>
-      </c>
-      <c r="B183" s="8">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="8">
-        <v>53.010033444816052</v>
-      </c>
-      <c r="B184" s="8">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="8">
-        <v>53.34448160535117</v>
-      </c>
-      <c r="B185" s="8">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="8">
-        <v>53.678929765886288</v>
-      </c>
-      <c r="B186" s="8">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="8">
-        <v>54.013377926421406</v>
-      </c>
-      <c r="B187" s="8">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="8">
-        <v>54.347826086956523</v>
-      </c>
-      <c r="B188" s="8">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="8">
-        <v>54.682274247491641</v>
-      </c>
-      <c r="B189" s="8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="8">
-        <v>55.016722408026759</v>
-      </c>
-      <c r="B190" s="8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="8">
-        <v>55.351170568561876</v>
-      </c>
-      <c r="B191" s="8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="8">
-        <v>55.685618729096987</v>
-      </c>
-      <c r="B192" s="8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="8">
-        <v>56.020066889632105</v>
-      </c>
-      <c r="B193" s="8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="8">
-        <v>56.354515050167223</v>
-      </c>
-      <c r="B194" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="8">
-        <v>56.68896321070234</v>
-      </c>
-      <c r="B195" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="8">
-        <v>57.023411371237458</v>
-      </c>
-      <c r="B196" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="8">
-        <v>57.357859531772576</v>
-      </c>
-      <c r="B197" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="8">
-        <v>57.692307692307693</v>
-      </c>
-      <c r="B198" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="8">
-        <v>58.026755852842811</v>
-      </c>
-      <c r="B199" s="8">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="8">
-        <v>58.361204013377929</v>
-      </c>
-      <c r="B200" s="8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="8">
-        <v>58.695652173913047</v>
-      </c>
-      <c r="B201" s="8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="8">
-        <v>59.030100334448164</v>
-      </c>
-      <c r="B202" s="8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="8">
-        <v>59.364548494983275</v>
-      </c>
-      <c r="B203" s="8">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="8">
-        <v>59.698996655518393</v>
-      </c>
-      <c r="B204" s="8">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="8">
-        <v>60.03344481605351</v>
-      </c>
-      <c r="B205" s="8">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="8">
-        <v>60.367892976588628</v>
-      </c>
-      <c r="B206" s="8">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="8">
-        <v>60.702341137123746</v>
-      </c>
-      <c r="B207" s="8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="8">
-        <v>61.036789297658864</v>
-      </c>
-      <c r="B208" s="8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="8">
-        <v>61.371237458193981</v>
-      </c>
-      <c r="B209" s="8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="8">
-        <v>61.705685618729099</v>
-      </c>
-      <c r="B210" s="8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="8">
-        <v>62.040133779264217</v>
-      </c>
-      <c r="B211" s="8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="8">
-        <v>62.374581939799334</v>
-      </c>
-      <c r="B212" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="8">
-        <v>62.709030100334445</v>
-      </c>
-      <c r="B213" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="8">
-        <v>63.043478260869563</v>
-      </c>
-      <c r="B214" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="8">
-        <v>63.37792642140468</v>
-      </c>
-      <c r="B215" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="8">
-        <v>63.712374581939798</v>
-      </c>
-      <c r="B216" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="8">
-        <v>64.046822742474916</v>
-      </c>
-      <c r="B217" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="8">
-        <v>64.381270903010034</v>
-      </c>
-      <c r="B218" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="8">
-        <v>64.715719063545151</v>
-      </c>
-      <c r="B219" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="8">
-        <v>65.050167224080269</v>
-      </c>
-      <c r="B220" s="8">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="8">
-        <v>65.384615384615387</v>
-      </c>
-      <c r="B221" s="8">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="8">
-        <v>65.719063545150505</v>
-      </c>
-      <c r="B222" s="8">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="8">
-        <v>66.053511705685622</v>
-      </c>
-      <c r="B223" s="8">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="8">
-        <v>66.38795986622074</v>
-      </c>
-      <c r="B224" s="8">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="8">
-        <v>66.722408026755858</v>
-      </c>
-      <c r="B225" s="8">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="8">
-        <v>67.056856187290975</v>
-      </c>
-      <c r="B226" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="8">
-        <v>67.391304347826093</v>
-      </c>
-      <c r="B227" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="8">
-        <v>67.725752508361211</v>
-      </c>
-      <c r="B228" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="8">
-        <v>68.060200668896314</v>
-      </c>
-      <c r="B229" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="8">
-        <v>68.394648829431432</v>
-      </c>
-      <c r="B230" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="8">
-        <v>68.72909698996655</v>
-      </c>
-      <c r="B231" s="8">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="8">
-        <v>69.063545150501668</v>
-      </c>
-      <c r="B232" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="8">
-        <v>69.397993311036785</v>
-      </c>
-      <c r="B233" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="8">
-        <v>69.732441471571903</v>
-      </c>
-      <c r="B234" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="8">
-        <v>70.066889632107021</v>
-      </c>
-      <c r="B235" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="8">
-        <v>70.401337792642138</v>
-      </c>
-      <c r="B236" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="8">
-        <v>70.735785953177256</v>
-      </c>
-      <c r="B237" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="8">
-        <v>71.070234113712374</v>
-      </c>
-      <c r="B238" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="8">
-        <v>71.404682274247492</v>
-      </c>
-      <c r="B239" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="8">
-        <v>71.739130434782609</v>
-      </c>
-      <c r="B240" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="8">
-        <v>72.073578595317727</v>
-      </c>
-      <c r="B241" s="8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="8">
-        <v>72.408026755852845</v>
-      </c>
-      <c r="B242" s="8">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="8">
-        <v>72.742474916387962</v>
-      </c>
-      <c r="B243" s="8">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="8">
-        <v>73.07692307692308</v>
-      </c>
-      <c r="B244" s="8">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="8">
-        <v>73.411371237458198</v>
-      </c>
-      <c r="B245" s="8">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="8">
-        <v>73.745819397993316</v>
-      </c>
-      <c r="B246" s="8">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="8">
-        <v>74.080267558528433</v>
-      </c>
-      <c r="B247" s="8">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="8">
-        <v>74.414715719063551</v>
-      </c>
-      <c r="B248" s="8">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="8">
-        <v>74.749163879598669</v>
-      </c>
-      <c r="B249" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="8">
-        <v>75.083612040133787</v>
-      </c>
-      <c r="B250" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="8">
-        <v>75.41806020066889</v>
-      </c>
-      <c r="B251" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="8">
-        <v>75.752508361204008</v>
-      </c>
-      <c r="B252" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="8">
-        <v>76.086956521739125</v>
-      </c>
-      <c r="B253" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="8">
-        <v>76.421404682274243</v>
-      </c>
-      <c r="B254" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="8">
-        <v>76.755852842809361</v>
-      </c>
-      <c r="B255" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="8">
-        <v>77.090301003344479</v>
-      </c>
-      <c r="B256" s="8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="8">
-        <v>77.424749163879596</v>
-      </c>
-      <c r="B257" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="8">
-        <v>77.759197324414714</v>
-      </c>
-      <c r="B258" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="8">
-        <v>78.093645484949832</v>
-      </c>
-      <c r="B259" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="8">
-        <v>78.42809364548495</v>
-      </c>
-      <c r="B260" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="8">
-        <v>78.762541806020067</v>
-      </c>
-      <c r="B261" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="8">
-        <v>79.096989966555185</v>
-      </c>
-      <c r="B262" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="8">
-        <v>79.431438127090303</v>
-      </c>
-      <c r="B263" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="8">
-        <v>79.76588628762542</v>
-      </c>
-      <c r="B264" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="8">
-        <v>80.100334448160538</v>
-      </c>
-      <c r="B265" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="8">
-        <v>80.434782608695656</v>
-      </c>
-      <c r="B266" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="8">
-        <v>80.769230769230774</v>
-      </c>
-      <c r="B267" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="8">
-        <v>81.103678929765891</v>
-      </c>
-      <c r="B268" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="8">
-        <v>81.438127090301009</v>
-      </c>
-      <c r="B269" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="8">
-        <v>81.772575250836127</v>
-      </c>
-      <c r="B270" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="8">
-        <v>82.107023411371244</v>
-      </c>
-      <c r="B271" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="8">
-        <v>82.441471571906348</v>
-      </c>
-      <c r="B272" s="8">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="8">
-        <v>82.775919732441466</v>
-      </c>
-      <c r="B273" s="8">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="8">
-        <v>83.110367892976583</v>
-      </c>
-      <c r="B274" s="8">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="8">
-        <v>83.444816053511701</v>
-      </c>
-      <c r="B275" s="8">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="8">
-        <v>83.779264214046819</v>
-      </c>
-      <c r="B276" s="8">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="8">
-        <v>84.113712374581937</v>
-      </c>
-      <c r="B277" s="8">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="8">
-        <v>84.448160535117054</v>
-      </c>
-      <c r="B278" s="8">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="8">
-        <v>84.782608695652172</v>
-      </c>
-      <c r="B279" s="8">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="8">
-        <v>85.11705685618729</v>
-      </c>
-      <c r="B280" s="8">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="8">
-        <v>85.451505016722408</v>
-      </c>
-      <c r="B281" s="8">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="8">
-        <v>85.785953177257525</v>
-      </c>
-      <c r="B282" s="8">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="8">
-        <v>86.120401337792643</v>
-      </c>
-      <c r="B283" s="8">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="8">
-        <v>86.454849498327761</v>
-      </c>
-      <c r="B284" s="8">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="8">
-        <v>86.789297658862878</v>
-      </c>
-      <c r="B285" s="8">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="8">
-        <v>87.123745819397996</v>
-      </c>
-      <c r="B286" s="8">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="8">
-        <v>87.458193979933114</v>
-      </c>
-      <c r="B287" s="8">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="8">
-        <v>87.792642140468232</v>
-      </c>
-      <c r="B288" s="8">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A289" s="8">
-        <v>88.127090301003349</v>
-      </c>
-      <c r="B289" s="8">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A290" s="8">
-        <v>88.461538461538467</v>
-      </c>
-      <c r="B290" s="8">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A291" s="8">
-        <v>88.795986622073585</v>
-      </c>
-      <c r="B291" s="8">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A292" s="8">
-        <v>89.130434782608702</v>
-      </c>
-      <c r="B292" s="8">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A293" s="8">
-        <v>89.464882943143806</v>
-      </c>
-      <c r="B293" s="8">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A294" s="8">
-        <v>89.799331103678924</v>
-      </c>
-      <c r="B294" s="8">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A295" s="8">
-        <v>90.133779264214041</v>
-      </c>
-      <c r="B295" s="8">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A296" s="8">
-        <v>90.468227424749159</v>
-      </c>
-      <c r="B296" s="8">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A297" s="8">
-        <v>90.802675585284277</v>
-      </c>
-      <c r="B297" s="8">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A298" s="8">
-        <v>91.137123745819395</v>
-      </c>
-      <c r="B298" s="8">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A299" s="8">
-        <v>91.471571906354512</v>
-      </c>
-      <c r="B299" s="8">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A300" s="8">
-        <v>91.80602006688963</v>
-      </c>
-      <c r="B300" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A301" s="8">
-        <v>92.140468227424748</v>
-      </c>
-      <c r="B301" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A302" s="8">
-        <v>92.474916387959865</v>
-      </c>
-      <c r="B302" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" s="8">
-        <v>92.809364548494983</v>
-      </c>
-      <c r="B303" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" s="8">
-        <v>93.143812709030101</v>
-      </c>
-      <c r="B304" s="8">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A305" s="8">
-        <v>93.478260869565219</v>
-      </c>
-      <c r="B305" s="8">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A306" s="8">
-        <v>93.812709030100336</v>
-      </c>
-      <c r="B306" s="8">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A307" s="8">
-        <v>94.147157190635454</v>
-      </c>
-      <c r="B307" s="8">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A308" s="8">
-        <v>94.481605351170572</v>
-      </c>
-      <c r="B308" s="8">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A309" s="8">
-        <v>94.81605351170569</v>
-      </c>
-      <c r="B309" s="8">
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A310" s="8">
-        <v>95.150501672240807</v>
-      </c>
-      <c r="B310" s="8">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A311" s="8">
-        <v>95.484949832775925</v>
-      </c>
-      <c r="B311" s="8">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A312" s="8">
-        <v>95.819397993311043</v>
-      </c>
-      <c r="B312" s="8">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A313" s="8">
-        <v>96.15384615384616</v>
-      </c>
-      <c r="B313" s="8">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A314" s="8">
-        <v>96.488294314381264</v>
-      </c>
-      <c r="B314" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A315" s="8">
-        <v>96.822742474916382</v>
-      </c>
-      <c r="B315" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A316" s="8">
-        <v>97.157190635451499</v>
-      </c>
-      <c r="B316" s="8">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A317" s="8">
-        <v>97.491638795986617</v>
-      </c>
-      <c r="B317" s="8">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A318" s="8">
-        <v>97.826086956521735</v>
-      </c>
-      <c r="B318" s="8">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A319" s="8">
-        <v>98.160535117056853</v>
-      </c>
-      <c r="B319" s="8">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A320" s="8">
-        <v>98.49498327759197</v>
-      </c>
-      <c r="B320" s="8">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A321" s="8">
-        <v>98.829431438127088</v>
-      </c>
-      <c r="B321" s="8">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A322" s="8">
-        <v>99.163879598662206</v>
-      </c>
-      <c r="B322" s="8">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A323" s="8">
-        <v>99.498327759197323</v>
-      </c>
-      <c r="B323" s="8">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A324" s="9">
-        <v>99.832775919732441</v>
-      </c>
-      <c r="B324" s="9">
-        <v>12.3</v>
+      <c r="B20" s="9">
+        <v>0.99800330026356043</v>
+      </c>
+      <c r="C20" s="9">
+        <v>7.6706582260483644E-2</v>
+      </c>
+      <c r="D20" s="9">
+        <v>13.01066050465521</v>
+      </c>
+      <c r="E20" s="9">
+        <v>6.4981658118298831E-31</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.84704392350121205</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1.1489626770259089</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.84704392350121205</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1.1489626770259089</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B26:B324">
-    <sortCondition ref="B26"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>